<commit_message>
Axiom 1, 2, 4, 3 tested / implemented
</commit_message>
<xml_diff>
--- a/30_LogicPaper_axioms.xlsx
+++ b/30_LogicPaper_axioms.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\LS510D3fc\admin\My Monolith\Origami\DIAMOND\DEFOX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long_\git\jyborg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8070" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="axioms" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="71">
   <si>
     <t>Axiom 5</t>
     <phoneticPr fontId="1"/>
@@ -127,14 +127,6 @@
   </si>
   <si>
     <t>n2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>|d1|</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>|d2|</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -313,6 +305,18 @@
     <t>* if</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>|d1|</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>|d2|</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -350,12 +354,18 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -398,7 +408,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -412,6 +422,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -577,11 +590,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81095280"/>
-        <c:axId val="-81092560"/>
+        <c:axId val="-47060336"/>
+        <c:axId val="-47074480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81095280"/>
+        <c:axId val="-47060336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -640,12 +653,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81092560"/>
+        <c:crossAx val="-47074480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81092560"/>
+        <c:axId val="-47074480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -704,7 +717,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81095280"/>
+        <c:crossAx val="-47060336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1073,11 +1086,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-81102352"/>
-        <c:axId val="-81791104"/>
+        <c:axId val="-47073936"/>
+        <c:axId val="-47067408"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-81102352"/>
+        <c:axId val="-47073936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1136,12 +1149,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81791104"/>
+        <c:crossAx val="-47067408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-81791104"/>
+        <c:axId val="-47067408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1200,7 +1213,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-81102352"/>
+        <c:crossAx val="-47073936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1270,6 +1283,76 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axiom3!$E$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axiom3!$F$20:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axiom3!$G$20:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
@@ -1301,110 +1384,30 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>axiom3!$C$56:$C$57</c:f>
+              <c:f>axiom3!$C$42:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>66.666666666666657</c:v>
+                  <c:v>-35.35533905932737</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>101356.56871158628</c:v>
+                  <c:v>-64.644660940672622</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>axiom3!$D$56:$D$57</c:f>
+              <c:f>axiom3!$D$42:$D$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>166.66666666666669</c:v>
+                  <c:v>64.644660940672622</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16603.75496920056</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>axiom3!$D$19</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>axiom3!$C$20:$C$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>axiom3!$D$20:$D$23</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>135.35533905932738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1443,30 +1446,602 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>axiom3!$C$65:$C$66</c:f>
+              <c:f>axiom3!$F$42:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>66.666666666666657</c:v>
+                  <c:v>-14.64466094067263</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16370.421635867226</c:v>
+                  <c:v>-85.355339059327378</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>axiom3!$D$65:$D$66</c:f>
+              <c:f>axiom3!$G$42:$G$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>166.66666666666669</c:v>
+                  <c:v>114.64466094067262</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-101456.56871158628</c:v>
+                  <c:v>85.355339059327378</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axioms!$B$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>the outline</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axioms!$C$41:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axioms!$D$41:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axiom3!$B$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axiom3!$C$20:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axiom3!$D$20:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-47063600"/>
+        <c:axId val="-47072304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-47063600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="-200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-47072304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-47072304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="200"/>
+          <c:min val="-200"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-47063600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axiom3!$B$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axiom3!$C$59:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-150</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axiom3!$D$59:$D$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axiom3!$E$59</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axiom3!$F$59:$F$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axiom3!$G$59:$G$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>axiom3!$B$69</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>p</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>axiom3!$C$69:$C$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>axiom3!$D$69:$D$70</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,11 +2144,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1861167952"/>
-        <c:axId val="-1861164144"/>
+        <c:axId val="-47073392"/>
+        <c:axId val="-47072848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1861167952"/>
+        <c:axId val="-47073392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1632,12 +2207,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861164144"/>
+        <c:crossAx val="-47072848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1861164144"/>
+        <c:axId val="-47072848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -1696,7 +2271,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861167952"/>
+        <c:crossAx val="-47073392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1745,7 +2320,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -1991,11 +2566,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1861165776"/>
-        <c:axId val="-1861165232"/>
+        <c:axId val="-47071760"/>
+        <c:axId val="-47070128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1861165776"/>
+        <c:axId val="-47071760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2054,12 +2629,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861165232"/>
+        <c:crossAx val="-47070128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1861165232"/>
+        <c:axId val="-47070128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2118,7 +2693,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861165776"/>
+        <c:crossAx val="-47071760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2167,7 +2742,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -2292,10 +2867,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-200</c:v>
+                  <c:v>-79</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2419,11 +2994,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1861173392"/>
-        <c:axId val="-1861166864"/>
+        <c:axId val="-47069584"/>
+        <c:axId val="-72452976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1861173392"/>
+        <c:axId val="-47069584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2482,12 +3057,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861166864"/>
+        <c:crossAx val="-72452976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1861166864"/>
+        <c:axId val="-72452976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2546,7 +3121,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861173392"/>
+        <c:crossAx val="-47069584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2595,7 +3170,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
@@ -2841,11 +3416,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1861163600"/>
-        <c:axId val="-1861168496"/>
+        <c:axId val="-1988575968"/>
+        <c:axId val="-1988573248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1861163600"/>
+        <c:axId val="-1988575968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2904,12 +3479,12 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861168496"/>
+        <c:crossAx val="-1988573248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1861168496"/>
+        <c:axId val="-1988573248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="200"/>
@@ -2968,7 +3543,7 @@
             <a:endParaRPr lang="ja-JP"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1861163600"/>
+        <c:crossAx val="-1988575968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3257,6 +3832,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5838,6 +6453,522 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -9870,11 +11001,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2438400" cy="1590676"/>
+    <xdr:ext cx="3276600" cy="1905000"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
@@ -9884,8 +11015,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="609600" y="7343775"/>
-              <a:ext cx="2438400" cy="1590676"/>
+              <a:off x="638175" y="6172200"/>
+              <a:ext cx="3276600" cy="1905000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -10006,7 +11137,7 @@
                                     <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                     </a:rPr>
-                                    <m:t>−</m:t>
+                                    <m:t>+</m:t>
                                   </m:r>
                                   <m:f>
                                     <m:fPr>
@@ -10078,7 +11209,7 @@
                                                 <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                                 </a:rPr>
-                                                <m:t>1</m:t>
+                                                <m:t>2</m:t>
                                               </m:r>
                                             </m:sub>
                                           </m:sSub>
@@ -10109,7 +11240,7 @@
                                                 <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                                 </a:rPr>
-                                                <m:t>2</m:t>
+                                                <m:t>1</m:t>
                                               </m:r>
                                             </m:sub>
                                           </m:sSub>
@@ -10246,7 +11377,7 @@
                                         <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         </a:rPr>
-                                        <m:t>−</m:t>
+                                        <m:t>+</m:t>
                                       </m:r>
                                       <m:f>
                                         <m:fPr>
@@ -10318,7 +11449,7 @@
                                                     <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                                     </a:rPr>
-                                                    <m:t>2</m:t>
+                                                    <m:t>1</m:t>
                                                   </m:r>
                                                 </m:sub>
                                               </m:sSub>
@@ -10349,7 +11480,7 @@
                                                     <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                                     </a:rPr>
-                                                    <m:t>1</m:t>
+                                                    <m:t>2</m:t>
                                                   </m:r>
                                                 </m:sub>
                                               </m:sSub>
@@ -10488,44 +11619,6 @@
                                     </a:rPr>
                                     <m:t>≔</m:t>
                                   </m:r>
-                                  <m:d>
-                                    <m:dPr>
-                                      <m:begChr m:val="|"/>
-                                      <m:endChr m:val="|"/>
-                                      <m:ctrlPr>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                        </a:rPr>
-                                      </m:ctrlPr>
-                                    </m:dPr>
-                                    <m:e>
-                                      <m:sSub>
-                                        <m:sSubPr>
-                                          <m:ctrlPr>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                            </a:rPr>
-                                          </m:ctrlPr>
-                                        </m:sSubPr>
-                                        <m:e>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                            </a:rPr>
-                                            <m:t>𝑑</m:t>
-                                          </m:r>
-                                        </m:e>
-                                        <m:sub>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                            </a:rPr>
-                                            <m:t>1</m:t>
-                                          </m:r>
-                                        </m:sub>
-                                      </m:sSub>
-                                    </m:e>
-                                  </m:d>
                                   <m:sSub>
                                     <m:sSubPr>
                                       <m:ctrlPr>
@@ -10557,44 +11650,95 @@
                                     </a:rPr>
                                     <m:t>+</m:t>
                                   </m:r>
-                                  <m:d>
-                                    <m:dPr>
-                                      <m:begChr m:val="|"/>
-                                      <m:endChr m:val="|"/>
+                                  <m:f>
+                                    <m:fPr>
                                       <m:ctrlPr>
                                         <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                         </a:rPr>
                                       </m:ctrlPr>
-                                    </m:dPr>
-                                    <m:e>
-                                      <m:sSub>
-                                        <m:sSubPr>
+                                    </m:fPr>
+                                    <m:num>
+                                      <m:d>
+                                        <m:dPr>
+                                          <m:begChr m:val="|"/>
+                                          <m:endChr m:val="|"/>
                                           <m:ctrlPr>
                                             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                               <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                             </a:rPr>
                                           </m:ctrlPr>
-                                        </m:sSubPr>
+                                        </m:dPr>
                                         <m:e>
-                                          <m:r>
+                                          <m:sSub>
+                                            <m:sSubPr>
+                                              <m:ctrlPr>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                              </m:ctrlPr>
+                                            </m:sSubPr>
+                                            <m:e>
+                                              <m:r>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                                <m:t>𝑑</m:t>
+                                              </m:r>
+                                            </m:e>
+                                            <m:sub>
+                                              <m:r>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                                <m:t>2</m:t>
+                                              </m:r>
+                                            </m:sub>
+                                          </m:sSub>
+                                        </m:e>
+                                      </m:d>
+                                    </m:num>
+                                    <m:den>
+                                      <m:d>
+                                        <m:dPr>
+                                          <m:begChr m:val="|"/>
+                                          <m:endChr m:val="|"/>
+                                          <m:ctrlPr>
                                             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
                                               <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                             </a:rPr>
-                                            <m:t>𝑑</m:t>
-                                          </m:r>
+                                          </m:ctrlPr>
+                                        </m:dPr>
+                                        <m:e>
+                                          <m:sSub>
+                                            <m:sSubPr>
+                                              <m:ctrlPr>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                              </m:ctrlPr>
+                                            </m:sSubPr>
+                                            <m:e>
+                                              <m:r>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                                <m:t>𝑑</m:t>
+                                              </m:r>
+                                            </m:e>
+                                            <m:sub>
+                                              <m:r>
+                                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
+                                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                                </a:rPr>
+                                                <m:t>1</m:t>
+                                              </m:r>
+                                            </m:sub>
+                                          </m:sSub>
                                         </m:e>
-                                        <m:sub>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1">
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                            </a:rPr>
-                                            <m:t>2</m:t>
-                                          </m:r>
-                                        </m:sub>
-                                      </m:sSub>
-                                    </m:e>
-                                  </m:d>
+                                      </m:d>
+                                    </m:den>
+                                  </m:f>
                                   <m:sSub>
                                     <m:sSubPr>
                                       <m:ctrlPr>
@@ -10707,8 +11851,8 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="609600" y="7343775"/>
-              <a:ext cx="2438400" cy="1590676"/>
+              <a:off x="638175" y="6172200"/>
+              <a:ext cx="3276600" cy="1905000"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -10740,11 +11884,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>{■8(█(𝑝≔𝑝_1−(𝑛_2⋅(𝑝_1−𝑝_2 ))/(𝑛_2⋅𝑑_1 ) 𝑑_1@(=𝑝_2−(𝑛_1⋅(𝑝_2−𝑝_1 ))/(𝑛_1⋅𝑑_2 ) 𝑑_2 ) )@█(𝑑^+≔|𝑑_1 | 𝑑_2+|𝑑_2 | 𝑑_1@𝑑^−≔𝜎𝑑^+ ))┤</a:t>
+                <a:t>{■8(█(𝑝≔𝑝_1+(𝑛_2⋅(𝑝_2−𝑝_1 ))/(𝑛_2⋅𝑑_1 ) 𝑑_1@(=𝑝_2+(𝑛_1⋅(𝑝_1−𝑝_2 ))/(𝑛_1⋅𝑑_2 ) 𝑑_2 ) )@█(𝑑^+≔𝑑_2+|𝑑_2 |/|𝑑_1 |  𝑑_1@𝑑^−≔𝜎𝑑^+ ))┤</a:t>
               </a:r>
               <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
             </a:p>
@@ -11185,16 +12330,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11217,9 +12362,9 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1247775" cy="361950"/>
@@ -11519,9 +12664,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>209551</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2438400" cy="1038224"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11533,7 +12678,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1190625" y="10058401"/>
+              <a:off x="1009650" y="15163801"/>
               <a:ext cx="2438400" cy="1038224"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -11637,77 +12782,6 @@
                                 </a:rPr>
                                 <m:t>≔</m:t>
                               </m:r>
-                              <m:sSub>
-                                <m:sSubPr>
-                                  <m:ctrlPr>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                  </m:ctrlPr>
-                                </m:sSubPr>
-                                <m:e>
-                                  <m:r>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>𝑝</m:t>
-                                  </m:r>
-                                </m:e>
-                                <m:sub>
-                                  <m:r>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>1</m:t>
-                                  </m:r>
-                                </m:sub>
-                              </m:sSub>
-                              <m:r>
-                                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                  <a:ln>
-                                    <a:noFill/>
-                                  </a:ln>
-                                  <a:solidFill>
-                                    <a:prstClr val="black"/>
-                                  </a:solidFill>
-                                  <a:effectLst/>
-                                  <a:uLnTx/>
-                                  <a:uFillTx/>
-                                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  <a:cs typeface="+mn-cs"/>
-                                </a:rPr>
-                                <m:t>+</m:t>
-                              </m:r>
                               <m:f>
                                 <m:fPr>
                                   <m:ctrlPr>
@@ -11760,243 +12834,7 @@
                                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
-                                        <m:t>𝑛</m:t>
-                                      </m:r>
-                                    </m:e>
-                                    <m:sub>
-                                      <m:r>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                          <a:ln>
-                                            <a:noFill/>
-                                          </a:ln>
-                                          <a:solidFill>
-                                            <a:prstClr val="black"/>
-                                          </a:solidFill>
-                                          <a:effectLst/>
-                                          <a:uLnTx/>
-                                          <a:uFillTx/>
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                          <a:cs typeface="+mn-cs"/>
-                                        </a:rPr>
-                                        <m:t>2</m:t>
-                                      </m:r>
-                                    </m:sub>
-                                  </m:sSub>
-                                  <m:r>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>⋅</m:t>
-                                  </m:r>
-                                  <m:d>
-                                    <m:dPr>
-                                      <m:ctrlPr>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                          <a:ln>
-                                            <a:noFill/>
-                                          </a:ln>
-                                          <a:solidFill>
-                                            <a:prstClr val="black"/>
-                                          </a:solidFill>
-                                          <a:effectLst/>
-                                          <a:uLnTx/>
-                                          <a:uFillTx/>
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                          <a:cs typeface="+mn-cs"/>
-                                        </a:rPr>
-                                      </m:ctrlPr>
-                                    </m:dPr>
-                                    <m:e>
-                                      <m:sSub>
-                                        <m:sSubPr>
-                                          <m:ctrlPr>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                          </m:ctrlPr>
-                                        </m:sSubPr>
-                                        <m:e>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                            <m:t>𝑝</m:t>
-                                          </m:r>
-                                        </m:e>
-                                        <m:sub>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                            <m:t>2</m:t>
-                                          </m:r>
-                                        </m:sub>
-                                      </m:sSub>
-                                      <m:r>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                          <a:ln>
-                                            <a:noFill/>
-                                          </a:ln>
-                                          <a:solidFill>
-                                            <a:prstClr val="black"/>
-                                          </a:solidFill>
-                                          <a:effectLst/>
-                                          <a:uLnTx/>
-                                          <a:uFillTx/>
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                          <a:cs typeface="+mn-cs"/>
-                                        </a:rPr>
-                                        <m:t>−</m:t>
-                                      </m:r>
-                                      <m:sSub>
-                                        <m:sSubPr>
-                                          <m:ctrlPr>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                          </m:ctrlPr>
-                                        </m:sSubPr>
-                                        <m:e>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                            <m:t>𝑝</m:t>
-                                          </m:r>
-                                        </m:e>
-                                        <m:sub>
-                                          <m:r>
-                                            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                              <a:ln>
-                                                <a:noFill/>
-                                              </a:ln>
-                                              <a:solidFill>
-                                                <a:prstClr val="black"/>
-                                              </a:solidFill>
-                                              <a:effectLst/>
-                                              <a:uLnTx/>
-                                              <a:uFillTx/>
-                                              <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                              <a:cs typeface="+mn-cs"/>
-                                            </a:rPr>
-                                            <m:t>1</m:t>
-                                          </m:r>
-                                        </m:sub>
-                                      </m:sSub>
-                                    </m:e>
-                                  </m:d>
-                                </m:num>
-                                <m:den>
-                                  <m:r>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>2</m:t>
-                                  </m:r>
-                                  <m:sSub>
-                                    <m:sSubPr>
-                                      <m:ctrlPr>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                          <a:ln>
-                                            <a:noFill/>
-                                          </a:ln>
-                                          <a:solidFill>
-                                            <a:prstClr val="black"/>
-                                          </a:solidFill>
-                                          <a:effectLst/>
-                                          <a:uLnTx/>
-                                          <a:uFillTx/>
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                          <a:cs typeface="+mn-cs"/>
-                                        </a:rPr>
-                                      </m:ctrlPr>
-                                    </m:sSubPr>
-                                    <m:e>
-                                      <m:r>
-                                        <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                          <a:ln>
-                                            <a:noFill/>
-                                          </a:ln>
-                                          <a:solidFill>
-                                            <a:prstClr val="black"/>
-                                          </a:solidFill>
-                                          <a:effectLst/>
-                                          <a:uLnTx/>
-                                          <a:uFillTx/>
-                                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                          <a:cs typeface="+mn-cs"/>
-                                        </a:rPr>
-                                        <m:t>𝑛</m:t>
+                                        <m:t>𝑝</m:t>
                                       </m:r>
                                     </m:e>
                                     <m:sub>
@@ -12032,7 +12870,7 @@
                                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
-                                    <m:t>⋅</m:t>
+                                    <m:t>+</m:t>
                                   </m:r>
                                   <m:sSub>
                                     <m:sSubPr>
@@ -12067,7 +12905,7 @@
                                           <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                           <a:cs typeface="+mn-cs"/>
                                         </a:rPr>
-                                        <m:t>𝑛</m:t>
+                                        <m:t>𝑝</m:t>
                                       </m:r>
                                     </m:e>
                                     <m:sub>
@@ -12089,27 +12927,8 @@
                                       </m:r>
                                     </m:sub>
                                   </m:sSub>
-                                </m:den>
-                              </m:f>
-                              <m:sSub>
-                                <m:sSubPr>
-                                  <m:ctrlPr>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                  </m:ctrlPr>
-                                </m:sSubPr>
-                                <m:e>
+                                </m:num>
+                                <m:den>
                                   <m:r>
                                     <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
                                       <a:ln>
@@ -12124,28 +12943,10 @@
                                       <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                                       <a:cs typeface="+mn-cs"/>
                                     </a:rPr>
-                                    <m:t>𝑑</m:t>
+                                    <m:t>2</m:t>
                                   </m:r>
-                                </m:e>
-                                <m:sub>
-                                  <m:r>
-                                    <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                                      <a:ln>
-                                        <a:noFill/>
-                                      </a:ln>
-                                      <a:solidFill>
-                                        <a:prstClr val="black"/>
-                                      </a:solidFill>
-                                      <a:effectLst/>
-                                      <a:uLnTx/>
-                                      <a:uFillTx/>
-                                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      <a:cs typeface="+mn-cs"/>
-                                    </a:rPr>
-                                    <m:t>1</m:t>
-                                  </m:r>
-                                </m:sub>
-                              </m:sSub>
+                                </m:den>
+                              </m:f>
                             </m:e>
                           </m:mr>
                           <m:mr>
@@ -12208,7 +13009,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="1190625" y="10058401"/>
+              <a:off x="1009650" y="15163801"/>
               <a:ext cx="2438400" cy="1038224"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -12262,7 +13063,7 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:rPr>
-                <a:t>𝑝≔𝑝_1+(𝑛_2⋅(𝑝_2−𝑝_1 ))/(2𝑛_1⋅𝑛_2 ) 𝑑_1@</a:t>
+                <a:t>𝑝≔(𝑝_1+𝑝_2)/2@</a:t>
               </a:r>
               <a:r>
                 <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" b="0" i="0">
@@ -12278,6 +13079,38 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="グラフ 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15039,7 +15872,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" thickTop="1" x14ac:dyDescent="0.15"/>
@@ -15055,12 +15888,12 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
@@ -15070,22 +15903,22 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C22" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
@@ -15095,27 +15928,27 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C30" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="C40" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>3</v>
@@ -15123,7 +15956,7 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C41" s="3">
         <f>SIZE</f>
@@ -15136,7 +15969,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B42" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C42" s="3">
         <f>-SIZE</f>
@@ -15149,7 +15982,7 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B43" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C43" s="3">
         <f>-SIZE</f>
@@ -15162,7 +15995,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B44" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C44" s="3">
         <f>SIZE</f>
@@ -15198,7 +16031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -15257,7 +16090,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="3">
         <f>SIZE</f>
@@ -15269,7 +16102,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="3">
         <v>0</v>
@@ -15280,7 +16113,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3">
         <f t="shared" ref="C23:D23" si="0">$C$21:$D$21+$C$25:$D$25</f>
@@ -15293,7 +16126,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="3">
         <f>SIZE/4</f>
@@ -15305,7 +16138,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C25" s="3">
         <v>0</v>
@@ -15317,7 +16150,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3">
         <f t="array" ref="C28:D28">C21:D21-C22:D22</f>
@@ -15329,7 +16162,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3">
         <f t="array" ref="C29:D29">C24:D24-C22:D22</f>
@@ -15396,7 +16229,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C56" s="3">
         <f t="shared" ref="C56:D56" si="1">$C$24:$D$24</f>
@@ -15409,7 +16242,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C57" s="3">
         <f t="shared" ref="C57:D57" si="2">C56:D56+C58:D58</f>
@@ -15422,7 +16255,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C58" s="3">
         <f>-$C$29:$D$29+$C$28:$D$28/2+$C$46/2*$C$25:$D$25</f>
@@ -15443,7 +16276,7 @@
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C62" s="3">
         <f t="shared" ref="C62:D62" si="3">$C$24:$D$24</f>
@@ -15456,7 +16289,7 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C63" s="3">
         <f t="shared" ref="C63:D63" si="4">C62:D62+C64:D64</f>
@@ -15469,7 +16302,7 @@
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C64" s="3">
         <f>-$C$29:$D$29+$C$28:$D$28/2+$C$47/2*$C$25:$D$25</f>
@@ -15490,15 +16323,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="5" width="9" style="1"/>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="9.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="7" width="9.375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="1"/>
   </cols>
@@ -15539,247 +16375,394 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
       <c r="C19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="F19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3">
+        <v>50</v>
+      </c>
+      <c r="D20" s="3">
+        <v>200</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="3">
+        <v>150</v>
+      </c>
+      <c r="G20" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="3">
-        <f>0</f>
+      <c r="C21" s="3">
+        <f>C20+C22</f>
         <v>0</v>
       </c>
-      <c r="D20" s="3">
-        <f>SIZE</f>
+      <c r="D21" s="3">
+        <f>D20+D22</f>
+        <v>150</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" s="3">
+        <f>F20+F22</f>
         <v>200</v>
       </c>
+      <c r="G21" s="3">
+        <f>G20+G22</f>
+        <v>100</v>
+      </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B21" s="3" t="s">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3">
+        <v>-50</v>
+      </c>
+      <c r="D22" s="3">
+        <v>-50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="3">
+        <v>50</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3">
+        <f>-D22</f>
+        <v>50</v>
+      </c>
+      <c r="D23" s="3">
+        <f>C22</f>
+        <v>-50</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="3">
+        <f>-G22</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <f>F22</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B37" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="3">
+        <f>SQRT(SUMPRODUCT($C$22:$D$22,$C$22:$D$22))</f>
+        <v>70.710678118654755</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B38" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="3">
+        <f>SQRT(SUMPRODUCT($F$22:$G$22,$F$22:$G$22))</f>
+        <v>50</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="3">
+        <f t="array" ref="C41:D41">$C$20:$D$20+SUMPRODUCT($F$23:$G$23,$F$20:$G$20-$C$20:$D$20)/SUMPRODUCT($F$23:$G$23,$C$22:$D$22)*$C$22:$D$22</f>
+        <v>-50</v>
+      </c>
+      <c r="D41" s="3">
+        <v>100</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="array" ref="F41:G41">C41:D41</f>
+        <v>-50</v>
+      </c>
+      <c r="G41" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="3">
+        <f>$C$41:$D$41+$C$44:$D$44</f>
+        <v>-35.35533905932737</v>
+      </c>
+      <c r="D42" s="3">
+        <f>$C$41:$D$41+$C$44:$D$44</f>
+        <v>64.644660940672622</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="array" ref="F42:G42">$F$41:$G$41+$F$44:$G$44</f>
+        <v>-14.64466094067263</v>
+      </c>
+      <c r="G42" s="3">
+        <v>114.64466094067262</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B43" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="3">
+        <f t="array" ref="C43:D43">$C$41:$D$41-$C$44:$D$44</f>
+        <v>-64.644660940672622</v>
+      </c>
+      <c r="D43" s="3">
+        <v>135.35533905932738</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="array" ref="F43:G43">$F$41:$G$41-$F$44:$G$44</f>
+        <v>-85.355339059327378</v>
+      </c>
+      <c r="G43" s="3">
+        <v>85.355339059327378</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="3">
+        <f t="array" ref="C44:D44">($F$22:$G$22+$C$38/$C$37*$C$22:$D$22)</f>
+        <v>14.64466094067263</v>
+      </c>
+      <c r="D44" s="3">
+        <v>-35.35533905932737</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="3">
+        <f>-$D$44</f>
+        <v>35.35533905932737</v>
+      </c>
+      <c r="G44" s="3">
+        <f>$C$44</f>
+        <v>14.64466094067263</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B48" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C59" s="3">
+        <v>-200</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F59" s="3">
+        <v>150</v>
+      </c>
+      <c r="G59" s="3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="array" ref="C60:D60">C61:D61+C59:D59</f>
+        <v>-150</v>
+      </c>
+      <c r="D60" s="3">
+        <v>-50</v>
+      </c>
+      <c r="E60" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="3">
-        <f t="shared" ref="C21:D21" si="0">$C$20:$D$20+$C$24:$D$24</f>
-        <v>200</v>
-      </c>
-      <c r="D21" s="3">
-        <f t="shared" si="0"/>
-        <v>100</v>
+      <c r="F60" s="3">
+        <f t="array" ref="F60:G60">F61:G61+F59:G59</f>
+        <v>184</v>
+      </c>
+      <c r="G60" s="3">
+        <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B22" s="3" t="s">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="3">
+        <v>50</v>
+      </c>
+      <c r="D61" s="3">
+        <v>-50</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F61" s="3">
+        <v>34</v>
+      </c>
+      <c r="G61" s="3">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="B62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" s="3">
+        <f>-D61</f>
+        <v>50</v>
+      </c>
+      <c r="D62" s="3">
+        <f>C61</f>
+        <v>50</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F62" s="3">
+        <f>-G61</f>
+        <v>34</v>
+      </c>
+      <c r="G62" s="3">
+        <f>F61</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.15">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C68" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B69" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="3">
-        <f>-SIZE/2</f>
-        <v>-100</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
+      <c r="C69" s="3">
+        <f t="array" ref="C69:D69">(C59:D59+F59:G59)/2</f>
+        <v>-25</v>
+      </c>
+      <c r="D69" s="3">
+        <v>25</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B23" s="3" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B70" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="3">
-        <f t="array" ref="C23:D23">$C$22:$D$22+$C$25:$D$25</f>
-        <v>100</v>
-      </c>
-      <c r="D23" s="3">
-        <v>200</v>
+      <c r="C70" s="3">
+        <f t="array" ref="C70:D70">C71:D71+C69:D69</f>
+        <v>25</v>
+      </c>
+      <c r="D70" s="3">
+        <v>-25</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="3">
-        <f>SIZE</f>
-        <v>200</v>
-      </c>
-      <c r="D24" s="3">
-        <f>-SIZE/2</f>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="3">
-        <f>SIZE</f>
-        <v>200</v>
-      </c>
-      <c r="D25" s="3">
-        <f>SIZE</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="3">
-        <f>-D24</f>
-        <v>100</v>
-      </c>
-      <c r="D29" s="3">
-        <f>C24</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="3">
-        <f>-D25</f>
-        <v>-200</v>
-      </c>
-      <c r="D30" s="3">
-        <f>C25</f>
-        <v>200</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.15">
-      <c r="C39" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B51" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C51" s="3">
-        <f>SQRT(SUMPRODUCT($C$24:$D$24,$C$24:$D$24))</f>
-        <v>223.60679774997897</v>
-      </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B52" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" s="3">
-        <f>SQRT(SUMPRODUCT($C$25:$D$25,$C$25:$D$25))</f>
-        <v>282.84271247461902</v>
-      </c>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C55" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B56" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C56" s="3">
-        <f>$C$20:$D$20-SUMPRODUCT($C$30:$D$30,$C$20:$D$20-$C$22:$D$22)/SUMPRODUCT($C$30:$D$30,$C$24:$D$24)*$C$24:$D$24</f>
-        <v>66.666666666666657</v>
-      </c>
-      <c r="D56" s="3">
-        <f>$C$20:$D$20-SUMPRODUCT($C$30:$D$30,$C$20:$D$20-$C$22:$D$22)/SUMPRODUCT($C$30:$D$30,$C$24:$D$24)*$C$24:$D$24</f>
-        <v>166.66666666666669</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B57" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" s="3">
-        <f t="shared" ref="C57:D57" si="1">$C$56:$D$56+$C$58:$D$58</f>
-        <v>101356.56871158628</v>
-      </c>
-      <c r="D57" s="3">
-        <f t="shared" si="1"/>
-        <v>16603.75496920056</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B58" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C58" s="3">
-        <f>$C$51*$C$25:$D$25+$C$52*$C$24:$D$24</f>
-        <v>101289.90204491961</v>
-      </c>
-      <c r="D58" s="3">
-        <f>$C$51*$C$25:$D$25+$C$52*$C$24:$D$24</f>
-        <v>16437.088302533892</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="C64" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B65" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="3">
-        <f>$C$20:$D$20-SUMPRODUCT($C$30:$D$30,$C$20:$D$20-$C$22:$D$22)/SUMPRODUCT($C$30:$D$30,$C$24:$D$24)*$C$24:$D$24</f>
-        <v>66.666666666666657</v>
-      </c>
-      <c r="D65" s="3">
-        <f>$C$20:$D$20-SUMPRODUCT($C$30:$D$30,$C$20:$D$20-$C$22:$D$22)/SUMPRODUCT($C$30:$D$30,$C$24:$D$24)*$C$24:$D$24</f>
-        <v>166.66666666666669</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B66" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66" s="3">
-        <f t="shared" ref="C66:D66" si="2">-$C$65:$D$65-$C$67:$D$67</f>
-        <v>16370.421635867226</v>
-      </c>
-      <c r="D66" s="3">
-        <f t="shared" si="2"/>
-        <v>-101456.56871158628</v>
-      </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B67" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="3">
-        <f>-$D$58</f>
-        <v>-16437.088302533892</v>
-      </c>
-      <c r="D67" s="3">
-        <f>$C$58</f>
-        <v>101289.90204491961</v>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B71" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="3">
+        <f t="array" ref="C71:D71">C61:D61</f>
+        <v>50</v>
+      </c>
+      <c r="D71" s="3">
+        <v>-50</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15787,7 +16770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -15798,7 +16781,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" thickTop="1" x14ac:dyDescent="0.15"/>
@@ -15832,7 +16815,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3">
         <f>0</f>
@@ -15845,7 +16828,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C25" s="3">
         <f>-SIZE</f>
@@ -15866,7 +16849,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C28" s="3">
         <f t="shared" ref="C28:D28" si="0">$C$25:$D$25-$C$24:$D$24</f>
@@ -15879,7 +16862,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29" s="3">
         <f>-D28</f>
@@ -15900,7 +16883,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="3">
         <f t="shared" ref="C32:D32" si="1">($C$24:$D$24+$C$25:$D$25)/2</f>
@@ -15913,7 +16896,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3">
         <f t="shared" ref="C33:D33" si="2">$C$32:$D$32+$C$34:$D$34</f>
@@ -15926,7 +16909,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C34" s="3">
         <f t="shared" ref="C34:D34" si="3">$C$29:$D$29</f>
@@ -15949,7 +16932,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
@@ -16002,34 +16985,32 @@
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="3">
-        <f>0</f>
-        <v>0</v>
-      </c>
-      <c r="D27" s="3">
-        <f>SIZE</f>
+      <c r="B27" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="5">
+        <v>121</v>
+      </c>
+      <c r="D27" s="5">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B28" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="3">
+      <c r="B28" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="5">
         <f t="shared" ref="C28:D28" si="0">$C$27:$D$27+$C$30:$D$30</f>
-        <v>-200</v>
-      </c>
-      <c r="D28" s="3">
+        <v>-79</v>
+      </c>
+      <c r="D28" s="5">
         <f t="shared" si="0"/>
         <v>-200</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29" s="3">
         <v>0</v>
@@ -16040,7 +17021,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C30" s="3">
         <f>-SIZE</f>
@@ -16061,7 +17042,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C33" s="3">
         <f>-D30</f>
@@ -16082,7 +17063,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C36" s="3">
         <f t="shared" ref="C36:D36" si="1">$C$29:$D$29</f>
@@ -16095,7 +17076,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C37" s="3">
         <f t="shared" ref="C37:D37" si="2">$C$36:$D$36+$C$38:$D$38</f>
@@ -16122,7 +17103,8 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16130,7 +17112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.15"/>
   <cols>
@@ -16139,7 +17121,7 @@
   <sheetData>
     <row r="1" spans="1:2" s="2" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" thickTop="1" x14ac:dyDescent="0.15"/>
@@ -16178,7 +17160,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3">
         <f>0</f>
@@ -16191,7 +17173,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3">
         <f>-SIZE/2</f>
@@ -16212,7 +17194,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="3">
         <f t="shared" ref="C26:D26" si="0">$C$23:$D$23-$C$22:$D$22</f>
@@ -16225,7 +17207,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C27" s="3">
         <f>-D26</f>
@@ -16246,7 +17228,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3">
         <f t="shared" ref="C30:D30" si="1">$C$23:$D$23</f>
@@ -16259,7 +17241,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B31" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3">
         <f t="shared" ref="C31:D31" si="2">$C$30:$D$30+$C$32:$D$32</f>

</xml_diff>